<commit_message>
Minor updates before first session.
</commit_message>
<xml_diff>
--- a/Session 2 - Matrices and image processing/Figures/Time to initialise matrix_tictoc.xlsx
+++ b/Session 2 - Matrices and image processing/Figures/Time to initialise matrix_tictoc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\Courses\MATLAB-course\Session 2 - Matrices and image processing\Figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Courses\MATLAB-course\Session 2 - Matrices and image processing\Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6698F5-F0EB-4F4E-A6E7-1B1744385845}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96310BB-5E74-40C4-8AD8-C7EBDBCEC793}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1920" windowWidth="16920" windowHeight="9468" xr2:uid="{F0EBB91F-5335-4000-A0C3-6A4963FC9CD9}"/>
+    <workbookView xWindow="1440" yWindow="390" windowWidth="18795" windowHeight="11835" xr2:uid="{F0EBB91F-5335-4000-A0C3-6A4963FC9CD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -94,7 +94,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -136,7 +136,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Resize</c:v>
+            <c:v>Resize matrix</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -184,9 +184,6 @@
                 <c:pt idx="5">
                   <c:v>9000000</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>12250000</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -197,25 +194,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.17</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.07</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.68</c:v>
+                  <c:v>2.88</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.95</c:v>
+                  <c:v>5.99</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.49</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>39.96</c:v>
+                  <c:v>10.64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -231,7 +225,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Zeros</c:v>
+            <c:v>Initialised</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -279,9 +273,6 @@
                 <c:pt idx="5">
                   <c:v>9000000</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>12250000</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -298,19 +289,16 @@
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.01</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.02</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.02</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.02</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -492,7 +480,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Time to initialise</a:t>
+                  <a:t>Time to process (s)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1179,16 +1167,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>678180</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>459105</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1516,18 +1504,18 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1541,122 +1529,101 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>500</v>
       </c>
       <c r="B2" s="2">
-        <f>A2*A2</f>
+        <f t="shared" ref="B2:B9" si="0">A2*A2</f>
         <v>250000</v>
       </c>
       <c r="C2">
-        <v>7.0000000000000007E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D2">
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1000</v>
       </c>
       <c r="B3" s="2">
-        <f>A3*A3</f>
+        <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
       <c r="C3">
-        <v>1.17</v>
+        <v>0.19</v>
       </c>
       <c r="D3">
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1500</v>
       </c>
       <c r="B4" s="2">
-        <f>A4*A4</f>
+        <f t="shared" si="0"/>
         <v>2250000</v>
       </c>
       <c r="C4">
-        <v>3.07</v>
+        <v>0.97</v>
       </c>
       <c r="D4">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2000</v>
       </c>
       <c r="B5" s="2">
-        <f>A5*A5</f>
+        <f t="shared" si="0"/>
         <v>4000000</v>
       </c>
       <c r="C5">
-        <v>6.68</v>
+        <v>2.88</v>
       </c>
       <c r="D5">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2500</v>
       </c>
       <c r="B6" s="2">
-        <f>A6*A6</f>
+        <f t="shared" si="0"/>
         <v>6250000</v>
       </c>
       <c r="C6">
-        <v>12.95</v>
+        <v>5.99</v>
       </c>
       <c r="D6">
-        <v>0.02</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3000</v>
       </c>
       <c r="B7" s="2">
-        <f>A7*A7</f>
+        <f t="shared" si="0"/>
         <v>9000000</v>
       </c>
       <c r="C7">
-        <v>23.49</v>
+        <v>10.64</v>
       </c>
       <c r="D7">
-        <v>0.02</v>
+        <v>0.11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>3500</v>
-      </c>
-      <c r="B8" s="2">
-        <f>A8*A8</f>
-        <v>12250000</v>
-      </c>
-      <c r="C8">
-        <v>39.96</v>
-      </c>
-      <c r="D8">
-        <v>0.02</v>
-      </c>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>30000</v>
-      </c>
-      <c r="B9" s="2">
-        <f>A9*A9</f>
-        <v>900000000</v>
-      </c>
-      <c r="D9">
-        <v>0.27</v>
-      </c>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C8">

</xml_diff>